<commit_message>
Update :  - When moving marker is allowed, could not open junction form (FrmVDKJuntion or FrmOPCJunction)
</commit_message>
<xml_diff>
--- a/wiki/Dia chi vung nho.xlsx
+++ b/wiki/Dia chi vung nho.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Thong so may tinh" sheetId="1" r:id="rId1"/>
-    <sheet name="Thong so chuong trinh" sheetId="2" r:id="rId2"/>
-    <sheet name="M0" sheetId="4" r:id="rId3"/>
-    <sheet name="S0" sheetId="5" r:id="rId4"/>
-    <sheet name="IO_List" sheetId="6" r:id="rId5"/>
-    <sheet name="IO_List_Nguoc" sheetId="7" r:id="rId6"/>
-    <sheet name="Y tuong cac ham" sheetId="3" r:id="rId7"/>
+    <sheet name="Chốt VDK" sheetId="8" r:id="rId1"/>
+    <sheet name="Thong so may tinh" sheetId="1" r:id="rId2"/>
+    <sheet name="Thong so chuong trinh" sheetId="2" r:id="rId3"/>
+    <sheet name="M0" sheetId="4" r:id="rId4"/>
+    <sheet name="S0" sheetId="5" r:id="rId5"/>
+    <sheet name="IO_List" sheetId="6" r:id="rId6"/>
+    <sheet name="IO_List_Nguoc" sheetId="7" r:id="rId7"/>
+    <sheet name="Y tuong cac ham" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1896" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="1256">
   <si>
     <t>YEAR_SP</t>
   </si>
@@ -3772,6 +3773,57 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Lý Tự Trọng - Hai Bà Trưng</t>
+  </si>
+  <si>
+    <t>Lý Tự Trọng - Đồng Khởi</t>
+  </si>
+  <si>
+    <t>Nguyễn Huệ - Lê Lợi Chốt 1 - 2</t>
+  </si>
+  <si>
+    <t>Nguyễn Huệ - Chốt 13</t>
+  </si>
+  <si>
+    <t>Tủ điều khiển</t>
+  </si>
+  <si>
+    <t>CPU 1</t>
+  </si>
+  <si>
+    <t>CPU 3</t>
+  </si>
+  <si>
+    <t>CPU 4</t>
+  </si>
+  <si>
+    <t>CPU 2</t>
+  </si>
+  <si>
+    <t>CPU 5</t>
+  </si>
+  <si>
+    <t>Nguyễn Huệ - Chốt 3
+Nguyễn Huệ - Chốt 7 - 8
+Nguyễn Huệ - Chốt 11 - 12</t>
+  </si>
+  <si>
+    <t>Nguyễn Huệ - Nguyễn Thiệp - Chốt 4
+Nguyễn Huệ - Chốt 9 - 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Huệ - Chốt 5 - 6 </t>
   </si>
 </sst>
 </file>
@@ -4102,7 +4154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4258,6 +4310,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4341,6 +4396,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:E10" totalsRowShown="0">
+  <autoFilter ref="B2:E10"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="STT"/>
+    <tableColumn id="2" name="Tên"/>
+    <tableColumn id="3" name="Port"/>
+    <tableColumn id="4" name="Tủ điều khiển"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4630,6 +4698,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1242</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D3">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D4">
+        <v>3101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D5">
+        <v>3102</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D6">
+        <v>3103</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D7">
+        <v>3104</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D8">
+        <v>3105</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D9">
+        <v>3106</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4849,7 +5046,7 @@
       <c r="F12" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G12" s="72" t="s">
+      <c r="G12" s="73" t="s">
         <v>814</v>
       </c>
       <c r="H12" s="46">
@@ -4875,7 +5072,7 @@
       <c r="F13" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G13" s="73"/>
+      <c r="G13" s="74"/>
       <c r="H13" s="46">
         <v>0</v>
       </c>
@@ -4899,7 +5096,7 @@
       <c r="F14" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G14" s="73"/>
+      <c r="G14" s="74"/>
       <c r="H14" s="46">
         <v>0</v>
       </c>
@@ -4923,7 +5120,7 @@
       <c r="F15" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G15" s="73"/>
+      <c r="G15" s="74"/>
       <c r="H15" s="46">
         <v>0</v>
       </c>
@@ -4947,7 +5144,7 @@
       <c r="F16" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G16" s="73"/>
+      <c r="G16" s="74"/>
       <c r="H16" s="46">
         <v>0</v>
       </c>
@@ -4971,7 +5168,7 @@
       <c r="F17" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G17" s="73"/>
+      <c r="G17" s="74"/>
       <c r="H17" s="46">
         <v>0</v>
       </c>
@@ -4995,7 +5192,7 @@
       <c r="F18" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G18" s="73"/>
+      <c r="G18" s="74"/>
       <c r="H18" s="46">
         <v>0</v>
       </c>
@@ -5019,7 +5216,7 @@
       <c r="F19" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G19" s="73"/>
+      <c r="G19" s="74"/>
       <c r="H19" s="46">
         <v>0</v>
       </c>
@@ -5043,7 +5240,7 @@
       <c r="F20" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G20" s="73"/>
+      <c r="G20" s="74"/>
       <c r="H20" s="46">
         <v>0</v>
       </c>
@@ -5067,7 +5264,7 @@
       <c r="F21" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G21" s="74"/>
+      <c r="G21" s="75"/>
       <c r="H21" s="46">
         <v>0</v>
       </c>
@@ -5091,7 +5288,7 @@
       <c r="F22" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G22" s="71" t="s">
+      <c r="G22" s="72" t="s">
         <v>271</v>
       </c>
       <c r="H22" s="46">
@@ -5117,7 +5314,7 @@
       <c r="F23" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G23" s="71"/>
+      <c r="G23" s="72"/>
       <c r="H23" s="46">
         <v>0</v>
       </c>
@@ -5141,7 +5338,7 @@
       <c r="F24" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G24" s="71"/>
+      <c r="G24" s="72"/>
       <c r="H24" s="46">
         <v>0</v>
       </c>
@@ -5165,7 +5362,7 @@
       <c r="F25" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G25" s="71"/>
+      <c r="G25" s="72"/>
       <c r="H25" s="46">
         <v>0</v>
       </c>
@@ -5189,7 +5386,7 @@
       <c r="F26" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G26" s="71"/>
+      <c r="G26" s="72"/>
       <c r="H26" s="46">
         <v>0</v>
       </c>
@@ -5213,7 +5410,7 @@
       <c r="F27" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G27" s="71"/>
+      <c r="G27" s="72"/>
       <c r="H27" s="46">
         <v>0</v>
       </c>
@@ -5237,7 +5434,7 @@
       <c r="F28" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G28" s="71" t="s">
+      <c r="G28" s="72" t="s">
         <v>272</v>
       </c>
       <c r="H28" s="46">
@@ -5263,7 +5460,7 @@
       <c r="F29" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G29" s="71"/>
+      <c r="G29" s="72"/>
       <c r="H29" s="46">
         <v>0</v>
       </c>
@@ -5287,7 +5484,7 @@
       <c r="F30" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G30" s="71"/>
+      <c r="G30" s="72"/>
       <c r="H30" s="46">
         <v>0</v>
       </c>
@@ -5311,7 +5508,7 @@
       <c r="F31" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G31" s="71"/>
+      <c r="G31" s="72"/>
       <c r="H31" s="46">
         <v>0</v>
       </c>
@@ -5335,7 +5532,7 @@
       <c r="F32" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G32" s="71"/>
+      <c r="G32" s="72"/>
       <c r="H32" s="46">
         <v>0</v>
       </c>
@@ -5359,7 +5556,7 @@
       <c r="F33" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G33" s="71"/>
+      <c r="G33" s="72"/>
       <c r="H33" s="46">
         <v>0</v>
       </c>
@@ -5383,7 +5580,7 @@
       <c r="F34" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G34" s="67" t="s">
+      <c r="G34" s="68" t="s">
         <v>298</v>
       </c>
       <c r="H34" s="46">
@@ -5409,7 +5606,7 @@
       <c r="F35" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G35" s="71"/>
+      <c r="G35" s="72"/>
       <c r="H35" s="46">
         <v>0</v>
       </c>
@@ -5433,7 +5630,7 @@
       <c r="F36" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G36" s="71"/>
+      <c r="G36" s="72"/>
       <c r="H36" s="46">
         <v>0</v>
       </c>
@@ -5457,7 +5654,7 @@
       <c r="F37" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G37" s="71"/>
+      <c r="G37" s="72"/>
       <c r="H37" s="46">
         <v>0</v>
       </c>
@@ -5481,7 +5678,7 @@
       <c r="F38" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G38" s="71"/>
+      <c r="G38" s="72"/>
       <c r="H38" s="46">
         <v>0</v>
       </c>
@@ -5505,7 +5702,7 @@
       <c r="F39" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G39" s="71"/>
+      <c r="G39" s="72"/>
       <c r="H39" s="46">
         <v>0</v>
       </c>
@@ -5529,7 +5726,7 @@
       <c r="F40" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G40" s="71" t="s">
+      <c r="G40" s="72" t="s">
         <v>273</v>
       </c>
       <c r="H40" s="46">
@@ -5555,7 +5752,7 @@
       <c r="F41" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G41" s="71"/>
+      <c r="G41" s="72"/>
       <c r="H41" s="46">
         <v>0</v>
       </c>
@@ -5579,7 +5776,7 @@
       <c r="F42" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G42" s="71"/>
+      <c r="G42" s="72"/>
       <c r="H42" s="46">
         <v>0</v>
       </c>
@@ -5603,7 +5800,7 @@
       <c r="F43" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G43" s="71"/>
+      <c r="G43" s="72"/>
       <c r="H43" s="46">
         <v>0</v>
       </c>
@@ -5627,7 +5824,7 @@
       <c r="F44" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G44" s="71"/>
+      <c r="G44" s="72"/>
       <c r="H44" s="46">
         <v>0</v>
       </c>
@@ -5651,7 +5848,7 @@
       <c r="F45" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G45" s="71"/>
+      <c r="G45" s="72"/>
       <c r="H45" s="46">
         <v>0</v>
       </c>
@@ -5675,7 +5872,7 @@
       <c r="F46" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G46" s="71" t="s">
+      <c r="G46" s="72" t="s">
         <v>274</v>
       </c>
       <c r="H46" s="46">
@@ -5701,7 +5898,7 @@
       <c r="F47" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G47" s="71"/>
+      <c r="G47" s="72"/>
       <c r="H47" s="46">
         <v>0</v>
       </c>
@@ -5725,7 +5922,7 @@
       <c r="F48" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G48" s="71"/>
+      <c r="G48" s="72"/>
       <c r="H48" s="46">
         <v>0</v>
       </c>
@@ -5749,7 +5946,7 @@
       <c r="F49" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G49" s="71"/>
+      <c r="G49" s="72"/>
       <c r="H49" s="46">
         <v>0</v>
       </c>
@@ -5773,7 +5970,7 @@
       <c r="F50" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G50" s="71"/>
+      <c r="G50" s="72"/>
       <c r="H50" s="46"/>
       <c r="I50" t="s">
         <v>1239</v>
@@ -5795,7 +5992,7 @@
       <c r="F51" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G51" s="71"/>
+      <c r="G51" s="72"/>
       <c r="H51" s="46">
         <v>0</v>
       </c>
@@ -5817,7 +6014,7 @@
         <v>1083</v>
       </c>
       <c r="F52" s="49"/>
-      <c r="G52" s="67" t="s">
+      <c r="G52" s="68" t="s">
         <v>281</v>
       </c>
       <c r="H52" s="49">
@@ -5841,7 +6038,7 @@
         <v>252</v>
       </c>
       <c r="F53" s="49"/>
-      <c r="G53" s="67"/>
+      <c r="G53" s="68"/>
       <c r="H53" s="49">
         <v>0</v>
       </c>
@@ -5863,7 +6060,7 @@
         <v>253</v>
       </c>
       <c r="F54" s="49"/>
-      <c r="G54" s="67"/>
+      <c r="G54" s="68"/>
       <c r="H54" s="49">
         <v>0</v>
       </c>
@@ -5885,7 +6082,7 @@
         <v>279</v>
       </c>
       <c r="F55" s="49"/>
-      <c r="G55" s="67"/>
+      <c r="G55" s="68"/>
       <c r="H55" s="49">
         <v>0</v>
       </c>
@@ -5909,7 +6106,7 @@
       <c r="F56" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G56" s="67"/>
+      <c r="G56" s="68"/>
       <c r="H56" s="46">
         <v>0</v>
       </c>
@@ -5931,7 +6128,7 @@
         <v>283</v>
       </c>
       <c r="F57" s="49"/>
-      <c r="G57" s="67" t="s">
+      <c r="G57" s="68" t="s">
         <v>282</v>
       </c>
       <c r="H57" s="49">
@@ -5955,7 +6152,7 @@
         <v>252</v>
       </c>
       <c r="F58" s="49"/>
-      <c r="G58" s="67"/>
+      <c r="G58" s="68"/>
       <c r="H58" s="49">
         <v>0</v>
       </c>
@@ -5977,7 +6174,7 @@
         <v>253</v>
       </c>
       <c r="F59" s="49"/>
-      <c r="G59" s="67"/>
+      <c r="G59" s="68"/>
       <c r="H59" s="49">
         <v>0</v>
       </c>
@@ -5999,7 +6196,7 @@
         <v>279</v>
       </c>
       <c r="F60" s="49"/>
-      <c r="G60" s="67"/>
+      <c r="G60" s="68"/>
       <c r="H60" s="49">
         <v>0</v>
       </c>
@@ -6023,7 +6220,7 @@
       <c r="F61" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G61" s="67"/>
+      <c r="G61" s="68"/>
       <c r="H61" s="46">
         <v>0</v>
       </c>
@@ -6045,7 +6242,7 @@
         <v>283</v>
       </c>
       <c r="F62" s="49"/>
-      <c r="G62" s="67" t="s">
+      <c r="G62" s="68" t="s">
         <v>285</v>
       </c>
       <c r="H62" s="49">
@@ -6069,7 +6266,7 @@
         <v>252</v>
       </c>
       <c r="F63" s="49"/>
-      <c r="G63" s="67"/>
+      <c r="G63" s="68"/>
       <c r="H63" s="49">
         <v>0</v>
       </c>
@@ -6091,7 +6288,7 @@
         <v>253</v>
       </c>
       <c r="F64" s="49"/>
-      <c r="G64" s="67"/>
+      <c r="G64" s="68"/>
       <c r="H64" s="49">
         <v>0</v>
       </c>
@@ -6113,7 +6310,7 @@
         <v>279</v>
       </c>
       <c r="F65" s="49"/>
-      <c r="G65" s="67"/>
+      <c r="G65" s="68"/>
       <c r="H65" s="49">
         <v>0</v>
       </c>
@@ -6137,7 +6334,7 @@
       <c r="F66" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G66" s="67"/>
+      <c r="G66" s="68"/>
       <c r="H66" s="46">
         <v>0</v>
       </c>
@@ -6159,7 +6356,7 @@
         <v>283</v>
       </c>
       <c r="F67" s="49"/>
-      <c r="G67" s="68" t="s">
+      <c r="G67" s="69" t="s">
         <v>286</v>
       </c>
       <c r="H67" s="49">
@@ -6183,7 +6380,7 @@
         <v>252</v>
       </c>
       <c r="F68" s="49"/>
-      <c r="G68" s="69"/>
+      <c r="G68" s="70"/>
       <c r="H68" s="49">
         <v>0</v>
       </c>
@@ -6205,7 +6402,7 @@
         <v>253</v>
       </c>
       <c r="F69" s="49"/>
-      <c r="G69" s="69"/>
+      <c r="G69" s="70"/>
       <c r="H69" s="49">
         <v>0</v>
       </c>
@@ -6227,7 +6424,7 @@
         <v>279</v>
       </c>
       <c r="F70" s="49"/>
-      <c r="G70" s="69"/>
+      <c r="G70" s="70"/>
       <c r="H70" s="49">
         <v>0</v>
       </c>
@@ -6251,7 +6448,7 @@
       <c r="F71" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G71" s="70"/>
+      <c r="G71" s="71"/>
       <c r="H71" s="46">
         <v>0</v>
       </c>
@@ -6273,7 +6470,7 @@
         <v>283</v>
       </c>
       <c r="F72" s="49"/>
-      <c r="G72" s="67" t="s">
+      <c r="G72" s="68" t="s">
         <v>287</v>
       </c>
       <c r="H72" s="49">
@@ -6297,7 +6494,7 @@
         <v>252</v>
       </c>
       <c r="F73" s="49"/>
-      <c r="G73" s="67"/>
+      <c r="G73" s="68"/>
       <c r="H73" s="49">
         <v>0</v>
       </c>
@@ -6319,7 +6516,7 @@
         <v>253</v>
       </c>
       <c r="F74" s="49"/>
-      <c r="G74" s="67"/>
+      <c r="G74" s="68"/>
       <c r="H74" s="49">
         <v>0</v>
       </c>
@@ -6341,7 +6538,7 @@
         <v>279</v>
       </c>
       <c r="F75" s="49"/>
-      <c r="G75" s="67"/>
+      <c r="G75" s="68"/>
       <c r="H75" s="49">
         <v>0</v>
       </c>
@@ -6365,7 +6562,7 @@
       <c r="F76" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G76" s="67"/>
+      <c r="G76" s="68"/>
       <c r="H76" s="46">
         <v>0</v>
       </c>
@@ -6387,7 +6584,7 @@
         <v>283</v>
       </c>
       <c r="F77" s="49"/>
-      <c r="G77" s="67" t="s">
+      <c r="G77" s="68" t="s">
         <v>288</v>
       </c>
       <c r="H77" s="49">
@@ -6411,7 +6608,7 @@
         <v>252</v>
       </c>
       <c r="F78" s="49"/>
-      <c r="G78" s="67"/>
+      <c r="G78" s="68"/>
       <c r="H78" s="49">
         <v>0</v>
       </c>
@@ -6433,7 +6630,7 @@
         <v>253</v>
       </c>
       <c r="F79" s="49"/>
-      <c r="G79" s="67"/>
+      <c r="G79" s="68"/>
       <c r="H79" s="49">
         <v>0</v>
       </c>
@@ -6455,7 +6652,7 @@
         <v>279</v>
       </c>
       <c r="F80" s="49"/>
-      <c r="G80" s="67"/>
+      <c r="G80" s="68"/>
       <c r="H80" s="49">
         <v>0</v>
       </c>
@@ -6479,7 +6676,7 @@
       <c r="F81" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G81" s="67"/>
+      <c r="G81" s="68"/>
       <c r="H81" s="46">
         <v>0</v>
       </c>
@@ -6501,7 +6698,7 @@
         <v>283</v>
       </c>
       <c r="F82" s="49"/>
-      <c r="G82" s="67" t="s">
+      <c r="G82" s="68" t="s">
         <v>289</v>
       </c>
       <c r="H82" s="49">
@@ -6525,7 +6722,7 @@
         <v>252</v>
       </c>
       <c r="F83" s="49"/>
-      <c r="G83" s="67"/>
+      <c r="G83" s="68"/>
       <c r="H83" s="49">
         <v>0</v>
       </c>
@@ -6547,7 +6744,7 @@
         <v>253</v>
       </c>
       <c r="F84" s="49"/>
-      <c r="G84" s="67"/>
+      <c r="G84" s="68"/>
       <c r="H84" s="49">
         <v>0</v>
       </c>
@@ -6569,7 +6766,7 @@
         <v>279</v>
       </c>
       <c r="F85" s="49"/>
-      <c r="G85" s="67"/>
+      <c r="G85" s="68"/>
       <c r="H85" s="49">
         <v>0</v>
       </c>
@@ -6593,7 +6790,7 @@
       <c r="F86" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G86" s="67"/>
+      <c r="G86" s="68"/>
       <c r="H86" s="46">
         <v>0</v>
       </c>
@@ -6615,7 +6812,7 @@
         <v>283</v>
       </c>
       <c r="F87" s="49"/>
-      <c r="G87" s="67" t="s">
+      <c r="G87" s="68" t="s">
         <v>291</v>
       </c>
       <c r="H87" s="49">
@@ -6639,7 +6836,7 @@
         <v>252</v>
       </c>
       <c r="F88" s="49"/>
-      <c r="G88" s="67"/>
+      <c r="G88" s="68"/>
       <c r="H88" s="49">
         <v>0</v>
       </c>
@@ -6661,7 +6858,7 @@
         <v>253</v>
       </c>
       <c r="F89" s="49"/>
-      <c r="G89" s="67"/>
+      <c r="G89" s="68"/>
       <c r="H89" s="49">
         <v>0</v>
       </c>
@@ -6683,7 +6880,7 @@
         <v>279</v>
       </c>
       <c r="F90" s="49"/>
-      <c r="G90" s="67"/>
+      <c r="G90" s="68"/>
       <c r="H90" s="49">
         <v>0</v>
       </c>
@@ -6707,7 +6904,7 @@
       <c r="F91" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G91" s="67"/>
+      <c r="G91" s="68"/>
       <c r="H91" s="46">
         <v>0</v>
       </c>
@@ -6729,7 +6926,7 @@
         <v>283</v>
       </c>
       <c r="F92" s="49"/>
-      <c r="G92" s="67" t="s">
+      <c r="G92" s="68" t="s">
         <v>292</v>
       </c>
       <c r="H92" s="49">
@@ -6753,7 +6950,7 @@
         <v>252</v>
       </c>
       <c r="F93" s="49"/>
-      <c r="G93" s="67"/>
+      <c r="G93" s="68"/>
       <c r="H93" s="49">
         <v>0</v>
       </c>
@@ -6775,7 +6972,7 @@
         <v>253</v>
       </c>
       <c r="F94" s="49"/>
-      <c r="G94" s="67"/>
+      <c r="G94" s="68"/>
       <c r="H94" s="49">
         <v>0</v>
       </c>
@@ -6797,7 +6994,7 @@
         <v>279</v>
       </c>
       <c r="F95" s="49"/>
-      <c r="G95" s="67"/>
+      <c r="G95" s="68"/>
       <c r="H95" s="49">
         <v>0</v>
       </c>
@@ -6821,7 +7018,7 @@
       <c r="F96" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G96" s="67"/>
+      <c r="G96" s="68"/>
       <c r="H96" s="46">
         <v>0</v>
       </c>
@@ -6843,7 +7040,7 @@
         <v>283</v>
       </c>
       <c r="F97" s="49"/>
-      <c r="G97" s="67" t="s">
+      <c r="G97" s="68" t="s">
         <v>293</v>
       </c>
       <c r="H97" s="49">
@@ -6867,7 +7064,7 @@
         <v>252</v>
       </c>
       <c r="F98" s="49"/>
-      <c r="G98" s="67"/>
+      <c r="G98" s="68"/>
       <c r="H98" s="49">
         <v>0</v>
       </c>
@@ -6889,7 +7086,7 @@
         <v>253</v>
       </c>
       <c r="F99" s="49"/>
-      <c r="G99" s="67"/>
+      <c r="G99" s="68"/>
       <c r="H99" s="49">
         <v>0</v>
       </c>
@@ -6911,7 +7108,7 @@
         <v>279</v>
       </c>
       <c r="F100" s="49"/>
-      <c r="G100" s="67"/>
+      <c r="G100" s="68"/>
       <c r="H100" s="49">
         <v>0</v>
       </c>
@@ -6935,7 +7132,7 @@
       <c r="F101" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G101" s="67"/>
+      <c r="G101" s="68"/>
       <c r="H101" s="46">
         <v>0</v>
       </c>
@@ -6957,7 +7154,7 @@
         <v>283</v>
       </c>
       <c r="F102" s="49"/>
-      <c r="G102" s="67" t="s">
+      <c r="G102" s="68" t="s">
         <v>294</v>
       </c>
       <c r="H102" s="49">
@@ -6981,7 +7178,7 @@
         <v>252</v>
       </c>
       <c r="F103" s="49"/>
-      <c r="G103" s="67"/>
+      <c r="G103" s="68"/>
       <c r="H103" s="49">
         <v>0</v>
       </c>
@@ -7003,7 +7200,7 @@
         <v>253</v>
       </c>
       <c r="F104" s="49"/>
-      <c r="G104" s="67"/>
+      <c r="G104" s="68"/>
       <c r="H104" s="49">
         <v>0</v>
       </c>
@@ -7025,7 +7222,7 @@
         <v>279</v>
       </c>
       <c r="F105" s="49"/>
-      <c r="G105" s="67"/>
+      <c r="G105" s="68"/>
       <c r="H105" s="49">
         <v>0</v>
       </c>
@@ -7049,7 +7246,7 @@
       <c r="F106" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G106" s="67"/>
+      <c r="G106" s="68"/>
       <c r="H106" s="46">
         <v>0</v>
       </c>
@@ -7071,7 +7268,7 @@
         <v>283</v>
       </c>
       <c r="F107" s="49"/>
-      <c r="G107" s="67" t="s">
+      <c r="G107" s="68" t="s">
         <v>295</v>
       </c>
       <c r="H107" s="49">
@@ -7095,7 +7292,7 @@
         <v>252</v>
       </c>
       <c r="F108" s="49"/>
-      <c r="G108" s="67"/>
+      <c r="G108" s="68"/>
       <c r="H108" s="49">
         <v>0</v>
       </c>
@@ -7117,7 +7314,7 @@
         <v>253</v>
       </c>
       <c r="F109" s="49"/>
-      <c r="G109" s="67"/>
+      <c r="G109" s="68"/>
       <c r="H109" s="49">
         <v>0</v>
       </c>
@@ -7139,7 +7336,7 @@
         <v>279</v>
       </c>
       <c r="F110" s="49"/>
-      <c r="G110" s="67"/>
+      <c r="G110" s="68"/>
       <c r="H110" s="49">
         <v>0</v>
       </c>
@@ -7163,7 +7360,7 @@
       <c r="F111" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G111" s="67"/>
+      <c r="G111" s="68"/>
       <c r="H111" s="46">
         <v>0</v>
       </c>
@@ -7185,7 +7382,7 @@
         <v>283</v>
       </c>
       <c r="F112" s="49"/>
-      <c r="G112" s="67" t="s">
+      <c r="G112" s="68" t="s">
         <v>296</v>
       </c>
       <c r="H112" s="49">
@@ -7209,7 +7406,7 @@
         <v>252</v>
       </c>
       <c r="F113" s="49"/>
-      <c r="G113" s="67"/>
+      <c r="G113" s="68"/>
       <c r="H113" s="49">
         <v>0</v>
       </c>
@@ -7231,7 +7428,7 @@
         <v>253</v>
       </c>
       <c r="F114" s="49"/>
-      <c r="G114" s="67"/>
+      <c r="G114" s="68"/>
       <c r="H114" s="49">
         <v>0</v>
       </c>
@@ -7253,7 +7450,7 @@
         <v>279</v>
       </c>
       <c r="F115" s="49"/>
-      <c r="G115" s="67"/>
+      <c r="G115" s="68"/>
       <c r="H115" s="49">
         <v>0</v>
       </c>
@@ -7277,7 +7474,7 @@
       <c r="F116" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="G116" s="67"/>
+      <c r="G116" s="68"/>
       <c r="H116" s="46">
         <v>0</v>
       </c>
@@ -7299,7 +7496,7 @@
         <v>283</v>
       </c>
       <c r="F117" s="49"/>
-      <c r="G117" s="67" t="s">
+      <c r="G117" s="68" t="s">
         <v>290</v>
       </c>
       <c r="H117" s="49">
@@ -7323,7 +7520,7 @@
         <v>252</v>
       </c>
       <c r="F118" s="49"/>
-      <c r="G118" s="67"/>
+      <c r="G118" s="68"/>
       <c r="H118" s="49">
         <v>0</v>
       </c>
@@ -7345,7 +7542,7 @@
         <v>253</v>
       </c>
       <c r="F119" s="49"/>
-      <c r="G119" s="67"/>
+      <c r="G119" s="68"/>
       <c r="H119" s="49">
         <v>0</v>
       </c>
@@ -7367,7 +7564,7 @@
         <v>279</v>
       </c>
       <c r="F120" s="49"/>
-      <c r="G120" s="67"/>
+      <c r="G120" s="68"/>
       <c r="H120" s="49">
         <v>0</v>
       </c>
@@ -7391,7 +7588,7 @@
       <c r="F121" s="53" t="s">
         <v>261</v>
       </c>
-      <c r="G121" s="72"/>
+      <c r="G121" s="73"/>
       <c r="H121" s="53">
         <v>0</v>
       </c>
@@ -7434,7 +7631,7 @@
         <v>1082</v>
       </c>
       <c r="F123" s="46"/>
-      <c r="G123" s="75" t="s">
+      <c r="G123" s="76" t="s">
         <v>917</v>
       </c>
       <c r="H123" s="46">
@@ -7458,7 +7655,7 @@
         <v>1082</v>
       </c>
       <c r="F124" s="46"/>
-      <c r="G124" s="76"/>
+      <c r="G124" s="77"/>
       <c r="H124" s="46">
         <v>0</v>
       </c>
@@ -7480,7 +7677,7 @@
         <v>1082</v>
       </c>
       <c r="F125" s="46"/>
-      <c r="G125" s="76"/>
+      <c r="G125" s="77"/>
       <c r="H125" s="46">
         <v>0</v>
       </c>
@@ -7502,7 +7699,7 @@
         <v>1082</v>
       </c>
       <c r="F126" s="46"/>
-      <c r="G126" s="76"/>
+      <c r="G126" s="77"/>
       <c r="H126" s="46">
         <v>0</v>
       </c>
@@ -7524,7 +7721,7 @@
         <v>1082</v>
       </c>
       <c r="F127" s="53"/>
-      <c r="G127" s="77"/>
+      <c r="G127" s="78"/>
       <c r="H127" s="53">
         <v>0</v>
       </c>
@@ -7600,7 +7797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H130"/>
   <sheetViews>
@@ -7652,7 +7849,7 @@
       </c>
       <c r="E3" s="64"/>
       <c r="F3" s="65"/>
-      <c r="G3" s="87" t="s">
+      <c r="G3" s="88" t="s">
         <v>379</v>
       </c>
       <c r="H3" t="s">
@@ -7671,7 +7868,7 @@
       </c>
       <c r="E4" s="51"/>
       <c r="F4" s="49"/>
-      <c r="G4" s="84"/>
+      <c r="G4" s="85"/>
       <c r="H4" t="s">
         <v>1239</v>
       </c>
@@ -7688,7 +7885,7 @@
       </c>
       <c r="E5" s="51"/>
       <c r="F5" s="49"/>
-      <c r="G5" s="84"/>
+      <c r="G5" s="85"/>
       <c r="H5" t="s">
         <v>1239</v>
       </c>
@@ -7705,7 +7902,7 @@
       </c>
       <c r="E6" s="51"/>
       <c r="F6" s="49"/>
-      <c r="G6" s="84"/>
+      <c r="G6" s="85"/>
       <c r="H6" t="s">
         <v>1239</v>
       </c>
@@ -7722,7 +7919,7 @@
       </c>
       <c r="E7" s="51"/>
       <c r="F7" s="49"/>
-      <c r="G7" s="84"/>
+      <c r="G7" s="85"/>
       <c r="H7" t="s">
         <v>1239</v>
       </c>
@@ -7739,7 +7936,7 @@
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="49"/>
-      <c r="G8" s="84"/>
+      <c r="G8" s="85"/>
       <c r="H8" t="s">
         <v>1239</v>
       </c>
@@ -7756,7 +7953,7 @@
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="38"/>
-      <c r="G9" s="85"/>
+      <c r="G9" s="86"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="45" t="s">
@@ -7770,7 +7967,7 @@
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="49"/>
-      <c r="G10" s="83" t="s">
+      <c r="G10" s="84" t="s">
         <v>377</v>
       </c>
       <c r="H10" t="s">
@@ -7789,7 +7986,7 @@
       </c>
       <c r="E11" s="51"/>
       <c r="F11" s="49"/>
-      <c r="G11" s="84"/>
+      <c r="G11" s="85"/>
       <c r="H11" t="s">
         <v>1239</v>
       </c>
@@ -7806,7 +8003,7 @@
       </c>
       <c r="E12" s="51"/>
       <c r="F12" s="49"/>
-      <c r="G12" s="84"/>
+      <c r="G12" s="85"/>
       <c r="H12" t="s">
         <v>1239</v>
       </c>
@@ -7823,7 +8020,7 @@
       </c>
       <c r="E13" s="51"/>
       <c r="F13" s="49"/>
-      <c r="G13" s="84"/>
+      <c r="G13" s="85"/>
       <c r="H13" t="s">
         <v>1239</v>
       </c>
@@ -7840,7 +8037,7 @@
       </c>
       <c r="E14" s="51"/>
       <c r="F14" s="49"/>
-      <c r="G14" s="84"/>
+      <c r="G14" s="85"/>
       <c r="H14" t="s">
         <v>1239</v>
       </c>
@@ -7857,7 +8054,7 @@
       </c>
       <c r="E15" s="51"/>
       <c r="F15" s="49"/>
-      <c r="G15" s="85"/>
+      <c r="G15" s="86"/>
       <c r="H15" t="s">
         <v>1239</v>
       </c>
@@ -7874,7 +8071,7 @@
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="78" t="s">
+      <c r="G16" s="79" t="s">
         <v>378</v>
       </c>
     </row>
@@ -7890,7 +8087,7 @@
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="86"/>
+      <c r="G17" s="87"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
@@ -7904,7 +8101,7 @@
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
-      <c r="G18" s="86"/>
+      <c r="G18" s="87"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
@@ -7918,7 +8115,7 @@
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="86"/>
+      <c r="G19" s="87"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
@@ -7932,7 +8129,7 @@
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="86"/>
+      <c r="G20" s="87"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -7946,7 +8143,7 @@
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="86"/>
+      <c r="G21" s="87"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
@@ -7960,7 +8157,7 @@
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="86"/>
+      <c r="G22" s="87"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
@@ -7974,7 +8171,7 @@
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="86"/>
+      <c r="G23" s="87"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
@@ -7988,7 +8185,7 @@
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="86"/>
+      <c r="G24" s="87"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
@@ -8002,7 +8199,7 @@
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="7"/>
-      <c r="G25" s="79"/>
+      <c r="G25" s="80"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
@@ -8051,7 +8248,7 @@
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="88" t="s">
+      <c r="G28" s="89" t="s">
         <v>378</v>
       </c>
     </row>
@@ -8067,7 +8264,7 @@
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="89"/>
+      <c r="G29" s="90"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
@@ -8121,7 +8318,7 @@
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="78" t="s">
+      <c r="G33" s="79" t="s">
         <v>393</v>
       </c>
     </row>
@@ -8137,7 +8334,7 @@
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="79"/>
+      <c r="G34" s="80"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
@@ -8245,7 +8442,7 @@
       <c r="D43" s="5"/>
       <c r="E43" s="6"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="78"/>
+      <c r="G43" s="79"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
@@ -8257,7 +8454,7 @@
       <c r="D44" s="5"/>
       <c r="E44" s="6"/>
       <c r="F44" s="7"/>
-      <c r="G44" s="79"/>
+      <c r="G44" s="80"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
@@ -8305,7 +8502,7 @@
       <c r="F47" s="7" t="s">
         <v>853</v>
       </c>
-      <c r="G47" s="78" t="s">
+      <c r="G47" s="79" t="s">
         <v>852</v>
       </c>
     </row>
@@ -8323,7 +8520,7 @@
       <c r="F48" s="7" t="s">
         <v>853</v>
       </c>
-      <c r="G48" s="79"/>
+      <c r="G48" s="80"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
@@ -8435,7 +8632,7 @@
       <c r="F55" s="7" t="s">
         <v>853</v>
       </c>
-      <c r="G55" s="78" t="s">
+      <c r="G55" s="79" t="s">
         <v>849</v>
       </c>
     </row>
@@ -8453,7 +8650,7 @@
       <c r="F56" s="7" t="s">
         <v>853</v>
       </c>
-      <c r="G56" s="79"/>
+      <c r="G56" s="80"/>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
@@ -8800,7 +8997,7 @@
       </c>
       <c r="E80" s="6"/>
       <c r="F80" s="7"/>
-      <c r="G80" s="78" t="s">
+      <c r="G80" s="79" t="s">
         <v>1184</v>
       </c>
     </row>
@@ -8816,7 +9013,7 @@
       </c>
       <c r="E81" s="6"/>
       <c r="F81" s="7"/>
-      <c r="G81" s="79"/>
+      <c r="G81" s="80"/>
     </row>
     <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="33" t="s">
@@ -8866,7 +9063,7 @@
       <c r="F85" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="G85" s="80" t="s">
+      <c r="G85" s="81" t="s">
         <v>1193</v>
       </c>
     </row>
@@ -8882,7 +9079,7 @@
       <c r="F86" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="G86" s="81"/>
+      <c r="G86" s="82"/>
     </row>
     <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="40" t="s">
@@ -8896,7 +9093,7 @@
       <c r="F87" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="G87" s="81"/>
+      <c r="G87" s="82"/>
     </row>
     <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" s="40" t="s">
@@ -8910,7 +9107,7 @@
       <c r="F88" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="G88" s="81"/>
+      <c r="G88" s="82"/>
     </row>
     <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="40" t="s">
@@ -8924,7 +9121,7 @@
       <c r="F89" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="G89" s="81"/>
+      <c r="G89" s="82"/>
     </row>
     <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="40" t="s">
@@ -8938,7 +9135,7 @@
       <c r="F90" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="G90" s="82"/>
+      <c r="G90" s="83"/>
     </row>
     <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" s="33" t="s">
@@ -9074,7 +9271,7 @@
       <c r="F103" s="43" t="s">
         <v>1192</v>
       </c>
-      <c r="G103" s="80" t="s">
+      <c r="G103" s="81" t="s">
         <v>1191</v>
       </c>
     </row>
@@ -9086,7 +9283,7 @@
       <c r="D104" s="41"/>
       <c r="E104" s="42"/>
       <c r="F104" s="43"/>
-      <c r="G104" s="81"/>
+      <c r="G104" s="82"/>
     </row>
     <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" s="40" t="s">
@@ -9102,7 +9299,7 @@
       <c r="F105" s="43" t="s">
         <v>1192</v>
       </c>
-      <c r="G105" s="81"/>
+      <c r="G105" s="82"/>
     </row>
     <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" s="40" t="s">
@@ -9112,7 +9309,7 @@
       <c r="D106" s="41"/>
       <c r="E106" s="42"/>
       <c r="F106" s="43"/>
-      <c r="G106" s="81"/>
+      <c r="G106" s="82"/>
     </row>
     <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" s="40" t="s">
@@ -9128,7 +9325,7 @@
       <c r="F107" s="43" t="s">
         <v>1192</v>
       </c>
-      <c r="G107" s="81"/>
+      <c r="G107" s="82"/>
     </row>
     <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" s="40" t="s">
@@ -9138,7 +9335,7 @@
       <c r="D108" s="41"/>
       <c r="E108" s="42"/>
       <c r="F108" s="43"/>
-      <c r="G108" s="81"/>
+      <c r="G108" s="82"/>
     </row>
     <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" s="40" t="s">
@@ -9154,7 +9351,7 @@
       <c r="F109" s="43" t="s">
         <v>1192</v>
       </c>
-      <c r="G109" s="81"/>
+      <c r="G109" s="82"/>
     </row>
     <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" s="40" t="s">
@@ -9164,7 +9361,7 @@
       <c r="D110" s="41"/>
       <c r="E110" s="42"/>
       <c r="F110" s="43"/>
-      <c r="G110" s="81"/>
+      <c r="G110" s="82"/>
     </row>
     <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" s="40" t="s">
@@ -9180,7 +9377,7 @@
       <c r="F111" s="43" t="s">
         <v>1192</v>
       </c>
-      <c r="G111" s="81"/>
+      <c r="G111" s="82"/>
     </row>
     <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="40" t="s">
@@ -9190,7 +9387,7 @@
       <c r="D112" s="41"/>
       <c r="E112" s="42"/>
       <c r="F112" s="43"/>
-      <c r="G112" s="81"/>
+      <c r="G112" s="82"/>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" s="40" t="s">
@@ -9206,7 +9403,7 @@
       <c r="F113" s="43" t="s">
         <v>1192</v>
       </c>
-      <c r="G113" s="82"/>
+      <c r="G113" s="83"/>
     </row>
     <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" s="33" t="s">
@@ -9397,7 +9594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H153"/>
   <sheetViews>
@@ -11375,11 +11572,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -13139,7 +13336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J23"/>
   <sheetViews>
@@ -13292,7 +13489,7 @@
       <c r="B6" s="29" t="s">
         <v>996</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="91" t="s">
         <v>1009</v>
       </c>
       <c r="E6" s="29">
@@ -13318,7 +13515,7 @@
       <c r="B7" s="29" t="s">
         <v>997</v>
       </c>
-      <c r="C7" s="90"/>
+      <c r="C7" s="91"/>
       <c r="E7" s="29">
         <v>1</v>
       </c>
@@ -13342,7 +13539,7 @@
       <c r="B8" s="29" t="s">
         <v>998</v>
       </c>
-      <c r="C8" s="90"/>
+      <c r="C8" s="91"/>
       <c r="E8" s="29">
         <v>1</v>
       </c>
@@ -13485,7 +13682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J23"/>
   <sheetViews>
@@ -13638,7 +13835,7 @@
       <c r="B6" s="29" t="s">
         <v>996</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="91" t="s">
         <v>1009</v>
       </c>
       <c r="E6" s="29">
@@ -13664,7 +13861,7 @@
       <c r="B7" s="29" t="s">
         <v>997</v>
       </c>
-      <c r="C7" s="90"/>
+      <c r="C7" s="91"/>
       <c r="E7" s="29">
         <v>1</v>
       </c>
@@ -13688,7 +13885,7 @@
       <c r="B8" s="29" t="s">
         <v>998</v>
       </c>
-      <c r="C8" s="90"/>
+      <c r="C8" s="91"/>
       <c r="E8" s="29">
         <v>1</v>
       </c>
@@ -13831,7 +14028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B18"/>
   <sheetViews>

</xml_diff>